<commit_message>
Carregando dados de out/2025
</commit_message>
<xml_diff>
--- a/upload/case-mix-2025.xlsx
+++ b/upload/case-mix-2025.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x17954399\OneDrive - FHEMIG\Coordenação de Informação - Geral\Portal de Dados Abertos MG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m10428324\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="13">
   <si>
     <t>unidade</t>
   </si>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:XFD85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -528,21 +528,21 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>1.4892000000000001</v>
+        <v>1.4527000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2">
         <v>2025</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>1.7827999999999999</v>
+        <v>1.5720000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -553,10 +553,10 @@
         <v>2025</v>
       </c>
       <c r="C12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>2.1297999999999999</v>
+        <v>1.7827999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -567,10 +567,10 @@
         <v>2025</v>
       </c>
       <c r="C13" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>2.4182999999999999</v>
+        <v>2.1297999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -581,10 +581,10 @@
         <v>2025</v>
       </c>
       <c r="C14" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>1.9123000000000001</v>
+        <v>2.4182999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -595,10 +595,10 @@
         <v>2025</v>
       </c>
       <c r="C15" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>1.6870000000000001</v>
+        <v>1.9123000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -609,10 +609,10 @@
         <v>2025</v>
       </c>
       <c r="C16" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>2.0131000000000001</v>
+        <v>1.6870000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -623,10 +623,10 @@
         <v>2025</v>
       </c>
       <c r="C17" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17">
-        <v>1.8540000000000001</v>
+        <v>2.0131000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -637,10 +637,10 @@
         <v>2025</v>
       </c>
       <c r="C18" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>2.1894999999999998</v>
+        <v>1.8540000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -651,38 +651,38 @@
         <v>2025</v>
       </c>
       <c r="C19" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>2.0306999999999999</v>
+        <v>2.1894999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>2025</v>
       </c>
       <c r="C20" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D20">
-        <v>0.94689999999999996</v>
+        <v>2.0306999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>2025</v>
       </c>
       <c r="C21" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>0.95220000000000005</v>
+        <v>2.3849</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -693,10 +693,10 @@
         <v>2025</v>
       </c>
       <c r="C22" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0.95209999999999995</v>
+        <v>0.94689999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -707,10 +707,10 @@
         <v>2025</v>
       </c>
       <c r="C23" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>1.0407999999999999</v>
+        <v>0.95220000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -721,10 +721,10 @@
         <v>2025</v>
       </c>
       <c r="C24" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>1.1008</v>
+        <v>0.95209999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -735,10 +735,10 @@
         <v>2025</v>
       </c>
       <c r="C25" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>1.0804</v>
+        <v>1.0407999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -749,10 +749,10 @@
         <v>2025</v>
       </c>
       <c r="C26" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>1.1073</v>
+        <v>1.1008</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -763,10 +763,10 @@
         <v>2025</v>
       </c>
       <c r="C27" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>0.98799999999999988</v>
+        <v>1.0804</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -777,52 +777,52 @@
         <v>2025</v>
       </c>
       <c r="C28" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>1.2061999999999999</v>
+        <v>1.1061000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="2">
         <v>2025</v>
       </c>
       <c r="C29" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D29">
-        <v>1.0690999999999999</v>
+        <v>0.98799999999999988</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2">
         <v>2025</v>
       </c>
       <c r="C30" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D30">
-        <v>1.0791999999999999</v>
+        <v>1.1752</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="2">
         <v>2025</v>
       </c>
       <c r="C31" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D31">
-        <v>1.206</v>
+        <v>0.89949999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -833,10 +833,10 @@
         <v>2025</v>
       </c>
       <c r="C32" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>1.1214999999999999</v>
+        <v>1.0690999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -847,10 +847,10 @@
         <v>2025</v>
       </c>
       <c r="C33" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>1.1617999999999999</v>
+        <v>1.0791999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -861,10 +861,10 @@
         <v>2025</v>
       </c>
       <c r="C34" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D34">
-        <v>0.64359999999999995</v>
+        <v>1.206</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -875,10 +875,10 @@
         <v>2025</v>
       </c>
       <c r="C35" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D35">
-        <v>1.3216000000000001</v>
+        <v>1.1214999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -889,10 +889,10 @@
         <v>2025</v>
       </c>
       <c r="C36" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D36">
-        <v>1.2175</v>
+        <v>1.1617999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -903,66 +903,66 @@
         <v>2025</v>
       </c>
       <c r="C37" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D37">
-        <v>1.1126</v>
+        <v>0.64359999999999995</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="2">
         <v>2025</v>
       </c>
       <c r="C38" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>1.7804</v>
+        <v>1.3216000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="2">
         <v>2025</v>
       </c>
       <c r="C39" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D39">
-        <v>1.673</v>
+        <v>1.2175</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="2">
         <v>2025</v>
       </c>
       <c r="C40" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D40">
-        <v>1.7311000000000001</v>
+        <v>1.1126</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" s="2">
         <v>2025</v>
       </c>
       <c r="C41" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D41">
-        <v>1.4615</v>
+        <v>1.1809000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -973,10 +973,10 @@
         <v>2025</v>
       </c>
       <c r="C42" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>1.4095</v>
+        <v>1.7804</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -987,10 +987,10 @@
         <v>2025</v>
       </c>
       <c r="C43" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D43">
-        <v>1.5999000000000001</v>
+        <v>1.6732</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1001,10 +1001,10 @@
         <v>2025</v>
       </c>
       <c r="C44" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>1.5866</v>
+        <v>1.7311000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1015,10 +1015,10 @@
         <v>2025</v>
       </c>
       <c r="C45" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>1.5329999999999999</v>
+        <v>1.4615</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1029,80 +1029,80 @@
         <v>2025</v>
       </c>
       <c r="C46" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D46">
-        <v>1.5177</v>
+        <v>1.4100999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" s="2">
         <v>2025</v>
       </c>
       <c r="C47" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D47">
-        <v>1.1957</v>
+        <v>1.5999000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="2">
         <v>2025</v>
       </c>
       <c r="C48" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D48">
-        <v>1.5170999999999999</v>
+        <v>1.5866</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" s="2">
         <v>2025</v>
       </c>
       <c r="C49" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D49">
-        <v>1.2679</v>
+        <v>1.5338000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" s="2">
         <v>2025</v>
       </c>
       <c r="C50" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D50">
-        <v>1.2907999999999999</v>
+        <v>1.5121</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" s="2">
         <v>2025</v>
       </c>
       <c r="C51" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D51">
-        <v>1.2582</v>
+        <v>1.4198</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1113,10 +1113,10 @@
         <v>2025</v>
       </c>
       <c r="C52" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <v>1.3304</v>
+        <v>1.1957</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1127,10 +1127,10 @@
         <v>2025</v>
       </c>
       <c r="C53" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D53">
-        <v>1.4404999999999999</v>
+        <v>1.5154999999999998</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1141,10 +1141,10 @@
         <v>2025</v>
       </c>
       <c r="C54" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D54">
-        <v>1.3317000000000001</v>
+        <v>1.2682</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1155,94 +1155,94 @@
         <v>2025</v>
       </c>
       <c r="C55" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D55">
-        <v>1.3179000000000001</v>
+        <v>1.2907999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B56" s="2">
         <v>2025</v>
       </c>
       <c r="C56" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D56">
-        <v>1.6221000000000001</v>
+        <v>1.2582</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57" s="2">
         <v>2025</v>
       </c>
       <c r="C57" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D57">
-        <v>1.7716000000000001</v>
+        <v>1.3306</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B58" s="2">
         <v>2025</v>
       </c>
       <c r="C58" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D58">
-        <v>1.7462</v>
+        <v>1.4404999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B59" s="2">
         <v>2025</v>
       </c>
       <c r="C59" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D59">
-        <v>1.9338000000000002</v>
+        <v>1.3319000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B60" s="2">
         <v>2025</v>
       </c>
       <c r="C60" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D60">
-        <v>1.9272</v>
+        <v>1.3179000000000001</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61" s="2">
         <v>2025</v>
       </c>
       <c r="C61" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D61">
-        <v>1.7902</v>
+        <v>1.4810000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1253,10 +1253,10 @@
         <v>2025</v>
       </c>
       <c r="C62" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>1.6865000000000001</v>
+        <v>1.6221000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1267,10 +1267,10 @@
         <v>2025</v>
       </c>
       <c r="C63" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D63">
-        <v>1.8592</v>
+        <v>1.7716000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1281,108 +1281,108 @@
         <v>2025</v>
       </c>
       <c r="C64" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D64">
-        <v>1.7318</v>
+        <v>1.7462</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65" s="2">
         <v>2025</v>
       </c>
       <c r="C65" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D65">
-        <v>0.94940000000000002</v>
+        <v>1.9338000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66" s="2">
         <v>2025</v>
       </c>
       <c r="C66" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D66">
-        <v>0.94810000000000005</v>
+        <v>1.9272</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67" s="2">
         <v>2025</v>
       </c>
       <c r="C67" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D67">
-        <v>1.0573999999999999</v>
+        <v>1.7902</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B68" s="2">
         <v>2025</v>
       </c>
       <c r="C68" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D68">
-        <v>1.1437999999999999</v>
+        <v>1.6865000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B69" s="2">
         <v>2025</v>
       </c>
       <c r="C69" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D69">
-        <v>0.97030000000000016</v>
+        <v>1.8592</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B70" s="2">
         <v>2025</v>
       </c>
       <c r="C70" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D70">
-        <v>1.0254000000000001</v>
+        <v>1.732</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B71" s="2">
         <v>2025</v>
       </c>
       <c r="C71" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D71">
-        <v>1.1004</v>
+        <v>2.1248999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1393,10 +1393,10 @@
         <v>2025</v>
       </c>
       <c r="C72" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>1.0247999999999999</v>
+        <v>0.94940000000000002</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1407,122 +1407,122 @@
         <v>2025</v>
       </c>
       <c r="C73" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D73">
-        <v>1.0640000000000001</v>
+        <v>0.94810000000000005</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B74" s="2">
         <v>2025</v>
       </c>
       <c r="C74" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D74">
-        <v>0.92949999999999999</v>
+        <v>1.0573999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" s="2">
         <v>2025</v>
       </c>
       <c r="C75" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D75">
-        <v>0.95120000000000016</v>
+        <v>1.1437999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B76" s="2">
         <v>2025</v>
       </c>
       <c r="C76" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D76">
-        <v>0.92459999999999998</v>
+        <v>0.97030000000000016</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77" s="2">
         <v>2025</v>
       </c>
       <c r="C77" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D77">
-        <v>0.85740000000000005</v>
+        <v>1.0254000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B78" s="2">
         <v>2025</v>
       </c>
       <c r="C78" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D78">
-        <v>0.91149999999999998</v>
+        <v>1.1004</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B79" s="2">
         <v>2025</v>
       </c>
       <c r="C79" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D79">
-        <v>0.89180000000000015</v>
+        <v>1.0247999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B80" s="2">
         <v>2025</v>
       </c>
       <c r="C80" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D80">
-        <v>0.92159999999999997</v>
+        <v>1.0640000000000001</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B81" s="2">
         <v>2025</v>
       </c>
       <c r="C81" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D81">
-        <v>0.97750000000000004</v>
+        <v>1.0622</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1533,278 +1533,139 @@
         <v>2025</v>
       </c>
       <c r="C82" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>0.91</v>
+        <v>0.92949999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C83" s="2">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>0.95120000000000016</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C84" s="2">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <v>0.92459999999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C85" s="2">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>0.85740000000000005</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C86" s="2">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>0.91149999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C87" s="2">
+        <v>6</v>
+      </c>
+      <c r="D87">
+        <v>0.89139999999999986</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C88" s="2">
+        <v>7</v>
+      </c>
+      <c r="D88">
+        <v>0.92159999999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C89" s="2">
+        <v>8</v>
+      </c>
+      <c r="D89">
+        <v>0.97750000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C90" s="2">
+        <v>9</v>
+      </c>
+      <c r="D90">
+        <v>0.91020000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C91" s="2">
+        <v>10</v>
+      </c>
+      <c r="D91">
+        <v>0.8950999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001F758B6196B0F49AC2B800DFBC943B3" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="d594503fc2142a00f6f31ee1b949d524">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee1baa49-d775-490f-95a0-0be6b1b30548" xmlns:ns3="0b0293c2-191e-4088-96c9-a881010ce1ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="38f63ce2bf38fd83141937b3be60016e" ns2:_="" ns3:_="">
-    <xsd:import namespace="ee1baa49-d775-490f-95a0-0be6b1b30548"/>
-    <xsd:import namespace="0b0293c2-191e-4088-96c9-a881010ce1ad"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ee1baa49-d775-490f-95a0-0be6b1b30548" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="7af98bd1-2354-4ddb-b15f-75f5f3c88b53" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0b0293c2-191e-4088-96c9-a881010ce1ad" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="17" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{31baf46e-eed5-4ebd-ba89-72a3afe19d19}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="0b0293c2-191e-4088-96c9-a881010ce1ad">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0b0293c2-191e-4088-96c9-a881010ce1ad" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee1baa49-d775-490f-95a0-0be6b1b30548">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68B741C0-251B-40F1-BD4F-F0C8AE7A2BDE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{107EB16A-4F9F-45C6-B803-CBAC3FD2CB98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ee1baa49-d775-490f-95a0-0be6b1b30548"/>
-    <ds:schemaRef ds:uri="0b0293c2-191e-4088-96c9-a881010ce1ad"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA51725D-29DF-4438-9DBE-BEFBC85C769F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ee1baa49-d775-490f-95a0-0be6b1b30548"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0b0293c2-191e-4088-96c9-a881010ce1ad"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>